<commit_message>
Corrected flipped RBWR and PBWR headers
</commit_message>
<xml_diff>
--- a/nfl-ol-stats.xlsx
+++ b/nfl-ol-stats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greghart/OneDrive/Development/Projects/NFLDraftData/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greghart/OneDrive/Development/Projects/NFLDraftData/position analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D305992-9701-584B-A1F4-F3EBE82D5CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59567513-CE7F-D04C-8E2D-B0747C8F47B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2760" windowWidth="27640" windowHeight="16940" xr2:uid="{0FC93A38-BA30-6D4D-AAEA-EBAF4F91EC80}"/>
   </bookViews>
@@ -724,7 +724,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -760,10 +760,10 @@
         <v>99</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>68</v>
@@ -813,15 +813,15 @@
         <v>67</v>
       </c>
       <c r="I2" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B2)</f>
+        <f t="shared" ref="I2:I33" si="1">_xlfn.PERCENTRANK.INC(B:B,B2)</f>
         <v>1</v>
       </c>
       <c r="J2" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C2)</f>
+        <f t="shared" ref="J2:J33" si="2">_xlfn.PERCENTRANK.INC(C:C,C2)</f>
         <v>1</v>
       </c>
       <c r="K2">
-        <f>B2+C2</f>
+        <f t="shared" ref="K2:K33" si="3">B2+C2</f>
         <v>148</v>
       </c>
       <c r="L2" s="3">
@@ -862,7 +862,7 @@
         <v>82.6</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F33" si="1">B3</f>
+        <f t="shared" ref="F3:F33" si="4">B3</f>
         <v>71</v>
       </c>
       <c r="G3" s="3">
@@ -874,19 +874,19 @@
         <v>60</v>
       </c>
       <c r="I3" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B3)</f>
+        <f t="shared" si="1"/>
         <v>0.96699999999999997</v>
       </c>
       <c r="J3" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C3)</f>
+        <f t="shared" si="2"/>
         <v>0.61199999999999999</v>
       </c>
       <c r="K3">
-        <f>B3+C3</f>
+        <f t="shared" si="3"/>
         <v>142</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L33" si="2">_xlfn.PERCENTRANK.INC(K:K,K3)</f>
+        <f t="shared" ref="L3:L33" si="5">_xlfn.PERCENTRANK.INC(K:K,K3)</f>
         <v>0.96699999999999997</v>
       </c>
       <c r="M3">
@@ -923,7 +923,7 @@
         <v>60.7</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="G4" s="3">
@@ -935,19 +935,19 @@
         <v>43</v>
       </c>
       <c r="I4" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B4)</f>
+        <f t="shared" si="1"/>
         <v>0.93500000000000005</v>
       </c>
       <c r="J4" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C4)</f>
+        <f t="shared" si="2"/>
         <v>0.70899999999999996</v>
       </c>
       <c r="K4">
-        <f>B4+C4</f>
+        <f t="shared" si="3"/>
         <v>139</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.93500000000000005</v>
       </c>
       <c r="M4">
@@ -984,7 +984,7 @@
         <v>69.599999999999994</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="G5" s="3">
@@ -996,19 +996,19 @@
         <v>43</v>
       </c>
       <c r="I5" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B5)</f>
+        <f t="shared" si="1"/>
         <v>0.90300000000000002</v>
       </c>
       <c r="J5" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C5)</f>
+        <f t="shared" si="2"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="K5">
-        <f>B5+C5</f>
+        <f t="shared" si="3"/>
         <v>133</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.77400000000000002</v>
       </c>
       <c r="M5">
@@ -1045,7 +1045,7 @@
         <v>74.3</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="G6" s="3">
@@ -1057,19 +1057,19 @@
         <v>59</v>
       </c>
       <c r="I6" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B6)</f>
+        <f t="shared" si="1"/>
         <v>0.80600000000000005</v>
       </c>
       <c r="J6" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C6)</f>
+        <f t="shared" si="2"/>
         <v>0.70899999999999996</v>
       </c>
       <c r="K6">
-        <f>B6+C6</f>
+        <f t="shared" si="3"/>
         <v>135</v>
       </c>
       <c r="L6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.87</v>
       </c>
       <c r="M6">
@@ -1106,7 +1106,7 @@
         <v>71</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="G7" s="3">
@@ -1118,19 +1118,19 @@
         <v>48</v>
       </c>
       <c r="I7" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B7)</f>
+        <f t="shared" si="1"/>
         <v>0.80600000000000005</v>
       </c>
       <c r="J7" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C7)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K7">
-        <f>B7+C7</f>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="L7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.61199999999999999</v>
       </c>
       <c r="M7">
@@ -1167,7 +1167,7 @@
         <v>78.7</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="G8" s="3">
@@ -1179,19 +1179,19 @@
         <v>37</v>
       </c>
       <c r="I8" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B8)</f>
+        <f t="shared" si="1"/>
         <v>0.80600000000000005</v>
       </c>
       <c r="J8" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C8)</f>
+        <f t="shared" si="2"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="K8">
-        <f>B8+C8</f>
+        <f t="shared" si="3"/>
         <v>133</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.77400000000000002</v>
       </c>
       <c r="M8">
@@ -1228,7 +1228,7 @@
         <v>69.8</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="G9" s="3">
@@ -1240,19 +1240,19 @@
         <v>59</v>
       </c>
       <c r="I9" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B9)</f>
+        <f t="shared" si="1"/>
         <v>0.74099999999999999</v>
       </c>
       <c r="J9" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C9)</f>
+        <f t="shared" si="2"/>
         <v>0.87</v>
       </c>
       <c r="K9">
-        <f>B9+C9</f>
+        <f t="shared" si="3"/>
         <v>135</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.87</v>
       </c>
       <c r="M9">
@@ -1289,7 +1289,7 @@
         <v>72.3</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="G10" s="3">
@@ -1301,19 +1301,19 @@
         <v>44</v>
       </c>
       <c r="I10" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B10)</f>
+        <f t="shared" si="1"/>
         <v>0.74099999999999999</v>
       </c>
       <c r="J10" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C10)</f>
+        <f t="shared" si="2"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="K10">
-        <f>B10+C10</f>
+        <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="L10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.67700000000000005</v>
       </c>
       <c r="M10">
@@ -1350,7 +1350,7 @@
         <v>59.3</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="G11" s="3">
@@ -1362,19 +1362,19 @@
         <v>48</v>
       </c>
       <c r="I11" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B11)</f>
+        <f t="shared" si="1"/>
         <v>0.64500000000000002</v>
       </c>
       <c r="J11" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C11)</f>
+        <f t="shared" si="2"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="K11">
-        <f>B11+C11</f>
+        <f t="shared" si="3"/>
         <v>129</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.51600000000000001</v>
       </c>
       <c r="M11">
@@ -1411,7 +1411,7 @@
         <v>67.099999999999994</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="G12" s="3">
@@ -1423,19 +1423,19 @@
         <v>35</v>
       </c>
       <c r="I12" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B12)</f>
+        <f t="shared" si="1"/>
         <v>0.64500000000000002</v>
       </c>
       <c r="J12" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C12)</f>
+        <f t="shared" si="2"/>
         <v>0.87</v>
       </c>
       <c r="K12">
-        <f>B12+C12</f>
+        <f t="shared" si="3"/>
         <v>133</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.77400000000000002</v>
       </c>
       <c r="M12">
@@ -1472,7 +1472,7 @@
         <v>79.2</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="G13" s="3">
@@ -1484,19 +1484,19 @@
         <v>56</v>
       </c>
       <c r="I13" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B13)</f>
+        <f t="shared" si="1"/>
         <v>0.64500000000000002</v>
       </c>
       <c r="J13" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C13)</f>
+        <f t="shared" si="2"/>
         <v>0.70899999999999996</v>
       </c>
       <c r="K13">
-        <f>B13+C13</f>
+        <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.67700000000000005</v>
       </c>
       <c r="M13">
@@ -1533,7 +1533,7 @@
         <v>76.2</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
       <c r="G14" s="3">
@@ -1545,19 +1545,19 @@
         <v>32</v>
       </c>
       <c r="I14" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B14)</f>
+        <f t="shared" si="1"/>
         <v>0.57999999999999996</v>
       </c>
       <c r="J14" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C14)</f>
+        <f t="shared" si="2"/>
         <v>0.70899999999999996</v>
       </c>
       <c r="K14">
-        <f>B14+C14</f>
+        <f t="shared" si="3"/>
         <v>131</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.64500000000000002</v>
       </c>
       <c r="M14">
@@ -1594,7 +1594,7 @@
         <v>71.5</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
       <c r="G15" s="3">
@@ -1606,19 +1606,19 @@
         <v>43</v>
       </c>
       <c r="I15" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B15)</f>
+        <f t="shared" si="1"/>
         <v>0.57999999999999996</v>
       </c>
       <c r="J15" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C15)</f>
+        <f t="shared" si="2"/>
         <v>0.87</v>
       </c>
       <c r="K15">
-        <f>B15+C15</f>
+        <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.67700000000000005</v>
       </c>
       <c r="M15">
@@ -1655,7 +1655,7 @@
         <v>69.5</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>57.999999999999993</v>
       </c>
       <c r="G16" s="3">
@@ -1667,19 +1667,19 @@
         <v>35</v>
       </c>
       <c r="I16" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B16)</f>
+        <f t="shared" si="1"/>
         <v>0.54800000000000004</v>
       </c>
       <c r="J16" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C16)</f>
+        <f t="shared" si="2"/>
         <v>0.61199999999999999</v>
       </c>
       <c r="K16">
-        <f>B16+C16</f>
+        <f t="shared" si="3"/>
         <v>129</v>
       </c>
       <c r="L16" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.51600000000000001</v>
       </c>
       <c r="M16">
@@ -1716,7 +1716,7 @@
         <v>64.099999999999994</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>56.999999999999993</v>
       </c>
       <c r="G17" s="3">
@@ -1728,19 +1728,19 @@
         <v>43</v>
       </c>
       <c r="I17" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B17)</f>
+        <f t="shared" si="1"/>
         <v>0.48299999999999998</v>
       </c>
       <c r="J17" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C17)</f>
+        <f t="shared" si="2"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="K17">
-        <f>B17+C17</f>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="L17" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.41899999999999998</v>
       </c>
       <c r="M17">
@@ -1777,7 +1777,7 @@
         <v>71.3</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>56.999999999999993</v>
       </c>
       <c r="G18" s="3">
@@ -1789,19 +1789,19 @@
         <v>55</v>
       </c>
       <c r="I18" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B18)</f>
+        <f t="shared" si="1"/>
         <v>0.48299999999999998</v>
       </c>
       <c r="J18" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C18)</f>
+        <f t="shared" si="2"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="K18">
-        <f>B18+C18</f>
+        <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="L18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.48299999999999998</v>
       </c>
       <c r="M18">
@@ -1838,7 +1838,7 @@
         <v>65.7</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>56.000000000000007</v>
       </c>
       <c r="G19" s="3">
@@ -1850,19 +1850,19 @@
         <v>45</v>
       </c>
       <c r="I19" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B19)</f>
+        <f t="shared" si="1"/>
         <v>0.41899999999999998</v>
       </c>
       <c r="J19" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C19)</f>
+        <f t="shared" si="2"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="K19">
-        <f>B19+C19</f>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="L19" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.41899999999999998</v>
       </c>
       <c r="M19">
@@ -1899,7 +1899,7 @@
         <v>59.3</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>56.000000000000007</v>
       </c>
       <c r="G20" s="3">
@@ -1911,19 +1911,19 @@
         <v>48</v>
       </c>
       <c r="I20" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B20)</f>
+        <f t="shared" si="1"/>
         <v>0.41899999999999998</v>
       </c>
       <c r="J20" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C20)</f>
+        <f t="shared" si="2"/>
         <v>0.87</v>
       </c>
       <c r="K20">
-        <f>B20+C20</f>
+        <f t="shared" si="3"/>
         <v>129</v>
       </c>
       <c r="L20" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.51600000000000001</v>
       </c>
       <c r="M20">
@@ -1960,7 +1960,7 @@
         <v>70.3</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>55.000000000000007</v>
       </c>
       <c r="G21" s="3">
@@ -1972,19 +1972,19 @@
         <v>44</v>
       </c>
       <c r="I21" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B21)</f>
+        <f t="shared" si="1"/>
         <v>0.38700000000000001</v>
       </c>
       <c r="J21" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C21)</f>
+        <f t="shared" si="2"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="K21">
-        <f>B21+C21</f>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="L21" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.35399999999999998</v>
       </c>
       <c r="M21">
@@ -2021,7 +2021,7 @@
         <v>58</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="G22" s="3">
@@ -2033,19 +2033,19 @@
         <v>37</v>
       </c>
       <c r="I22" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B22)</f>
+        <f t="shared" si="1"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="J22" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C22)</f>
+        <f t="shared" si="2"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="K22">
-        <f>B22+C22</f>
+        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="L22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="M22">
@@ -2082,7 +2082,7 @@
         <v>81</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="G23" s="3">
@@ -2094,19 +2094,19 @@
         <v>38</v>
       </c>
       <c r="I23" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B23)</f>
+        <f t="shared" si="1"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="J23" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C23)</f>
+        <f t="shared" si="2"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="K23">
-        <f>B23+C23</f>
+        <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="L23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.25800000000000001</v>
       </c>
       <c r="M23">
@@ -2143,7 +2143,7 @@
         <v>65.400000000000006</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
       <c r="G24" s="3">
@@ -2155,19 +2155,19 @@
         <v>43</v>
       </c>
       <c r="I24" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B24)</f>
+        <f t="shared" si="1"/>
         <v>0.25800000000000001</v>
       </c>
       <c r="J24" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C24)</f>
+        <f t="shared" si="2"/>
         <v>0.70899999999999996</v>
       </c>
       <c r="K24">
-        <f>B24+C24</f>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="L24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.35399999999999998</v>
       </c>
       <c r="M24">
@@ -2204,7 +2204,7 @@
         <v>77.8</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
       <c r="G25" s="3">
@@ -2216,19 +2216,19 @@
         <v>52</v>
       </c>
       <c r="I25" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B25)</f>
+        <f t="shared" si="1"/>
         <v>0.25800000000000001</v>
       </c>
       <c r="J25" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C25)</f>
+        <f t="shared" si="2"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="K25">
-        <f>B25+C25</f>
+        <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="L25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.25800000000000001</v>
       </c>
       <c r="M25">
@@ -2275,19 +2275,19 @@
         <v>33</v>
       </c>
       <c r="I26" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B26)</f>
+        <f t="shared" si="1"/>
         <v>0.129</v>
       </c>
       <c r="J26" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C26)</f>
+        <f t="shared" si="2"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="K26">
-        <f>B26+C26</f>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="L26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="M26">
@@ -2324,7 +2324,7 @@
         <v>57.2</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>51</v>
       </c>
       <c r="G27" s="3">
@@ -2336,19 +2336,19 @@
         <v>43</v>
       </c>
       <c r="I27" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B27)</f>
+        <f t="shared" si="1"/>
         <v>0.129</v>
       </c>
       <c r="J27" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C27)</f>
+        <f t="shared" si="2"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="K27">
-        <f>B27+C27</f>
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="L27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.193</v>
       </c>
       <c r="M27">
@@ -2385,7 +2385,7 @@
         <v>55.9</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>51</v>
       </c>
       <c r="G28" s="3">
@@ -2397,19 +2397,19 @@
         <v>39</v>
       </c>
       <c r="I28" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B28)</f>
+        <f t="shared" si="1"/>
         <v>0.129</v>
       </c>
       <c r="J28" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C28)</f>
+        <f t="shared" si="2"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="K28">
-        <f>B28+C28</f>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="L28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="M28">
@@ -2456,19 +2456,19 @@
         <v>42</v>
       </c>
       <c r="I29" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B29)</f>
+        <f t="shared" si="1"/>
         <v>0.129</v>
       </c>
       <c r="J29" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C29)</f>
+        <f t="shared" si="2"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="K29">
-        <f>B29+C29</f>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="L29" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="M29">
@@ -2505,7 +2505,7 @@
         <v>65</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="G30" s="3">
@@ -2517,19 +2517,19 @@
         <v>31</v>
       </c>
       <c r="I30" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B30)</f>
+        <f t="shared" si="1"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="J30" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C30)</f>
+        <f t="shared" si="2"/>
         <v>0.61199999999999999</v>
       </c>
       <c r="K30">
-        <f>B30+C30</f>
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="L30" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.193</v>
       </c>
       <c r="M30">
@@ -2566,7 +2566,7 @@
         <v>65.2</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="G31" s="3">
@@ -2578,19 +2578,19 @@
         <v>25</v>
       </c>
       <c r="I31" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B31)</f>
+        <f t="shared" si="1"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="J31" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K31">
-        <f>B31+C31</f>
+        <f t="shared" si="3"/>
         <v>117</v>
       </c>
       <c r="L31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="M31">
@@ -2627,7 +2627,7 @@
         <v>46.5</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="G32" s="3">
@@ -2639,19 +2639,19 @@
         <v>43</v>
       </c>
       <c r="I32" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B32)</f>
+        <f t="shared" si="1"/>
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="J32" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C32)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K32">
-        <f>B32+C32</f>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="L32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M32">
@@ -2688,7 +2688,7 @@
         <v>62.5</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
       <c r="G33" s="3">
@@ -2700,19 +2700,19 @@
         <v>32</v>
       </c>
       <c r="I33" s="3">
-        <f>_xlfn.PERCENTRANK.INC(B:B,B33)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J33" s="3">
-        <f>_xlfn.PERCENTRANK.INC(C:C,C33)</f>
+        <f t="shared" si="2"/>
         <v>0.32200000000000001</v>
       </c>
       <c r="K33">
-        <f>B33+C33</f>
+        <f t="shared" si="3"/>
         <v>116</v>
       </c>
       <c r="L33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="M33">

</xml_diff>